<commit_message>
alteração ordem de colunas no relatório de horas consolidado
</commit_message>
<xml_diff>
--- a/src/pause-web/src/main/resources/QA360.xlsx
+++ b/src/pause-web/src/main/resources/QA360.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilherme.oliveira\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\regpontov2\src\pause-web\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -199,37 +199,37 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,7 +602,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F30"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -610,270 +610,269 @@
     <col min="1" max="1" width="40.42578125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" ht="15.75">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="3"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="6" spans="1:6" ht="16.5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="16.5">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="16.5">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="16.5">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="16.5">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="16.5">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="16.5">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" ht="16.5">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="16.5">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" ht="16.5">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" ht="16.5">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" ht="16.5">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="16.5">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" ht="16.5">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" ht="16.5">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" ht="16.5">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" ht="16.5">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" ht="16.5">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" ht="16.5">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="16.5">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" ht="16.5">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6" ht="16.5">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" ht="16.5">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" ht="16.5">
-      <c r="A29" s="9"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
correção ordem de colunas no modelo de relatório consolidado (Verity e QA360)
</commit_message>
<xml_diff>
--- a/src/pause-web/src/main/resources/QA360.xlsx
+++ b/src/pause-web/src/main/resources/QA360.xlsx
@@ -659,10 +659,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>9</v>

</xml_diff>